<commit_message>
Adding Rows Error Fixed
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -64,12 +64,6 @@
     <t>Open</t>
   </si>
   <si>
-    <t>Bryce</t>
-  </si>
-  <si>
-    <t>Whasd</t>
-  </si>
-  <si>
     <t>Climber</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
   </si>
   <si>
     <t>Lydia Heydlauff</t>
-  </si>
-  <si>
-    <t>Bryce Whasd</t>
   </si>
 </sst>
 </file>
@@ -411,13 +402,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -468,8 +459,11 @@
       <c r="J2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -497,23 +491,11 @@
       <c r="J3">
         <v>180</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
+      <c r="K3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="G4">
         <v>3</v>
       </c>
@@ -525,6 +507,26 @@
       </c>
       <c r="J4">
         <v>280</v>
+      </c>
+      <c r="K4">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>400</v>
+      </c>
+      <c r="I5">
+        <v>390</v>
+      </c>
+      <c r="J5">
+        <v>380</v>
+      </c>
+      <c r="K5">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -534,76 +536,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -611,7 +544,71 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>17</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -625,47 +622,42 @@
       <c r="E1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>760</v>
+        <v>1340</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>280</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>1330</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
+        <v>1820</v>
       </c>
       <c r="D3">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>1420</v>
-      </c>
-      <c r="C4">
-        <v>90</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>